<commit_message>
implement shift and check10 logic
</commit_message>
<xml_diff>
--- a/50002_1d/mojo pinout ref.xlsx
+++ b/50002_1d/mojo pinout ref.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Desktop\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\School\github repos\50.002\50002_1d\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>gnd</t>
   </si>
@@ -111,6 +111,24 @@
   </si>
   <si>
     <t>io dip</t>
+  </si>
+  <si>
+    <t>display_select</t>
+  </si>
+  <si>
+    <t>display_digit</t>
+  </si>
+  <si>
+    <t>arrow_btn</t>
+  </si>
+  <si>
+    <t>start_game</t>
+  </si>
+  <si>
+    <t>win_led</t>
+  </si>
+  <si>
+    <t>lose_led</t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -193,28 +211,535 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AA22"/>
+  <dimension ref="A3:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -542,368 +1067,371 @@
     <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>51</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="3">
         <v>41</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="3">
         <v>35</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="3">
         <v>33</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="3">
         <v>30</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="3">
         <v>27</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="4">
         <v>24</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="4">
         <v>22</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="4">
         <v>17</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="4">
         <v>15</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="16">
         <v>12</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="16">
         <v>10</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="17">
         <v>8</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="17">
         <v>6</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="17">
         <v>2</v>
       </c>
-      <c r="T3" s="10">
+      <c r="T3" s="17">
         <v>144</v>
       </c>
-      <c r="U3" s="15">
+      <c r="U3" s="18">
         <v>142</v>
       </c>
-      <c r="V3" s="15">
+      <c r="V3" s="18">
         <v>140</v>
       </c>
-      <c r="W3" s="15">
+      <c r="W3" s="18">
         <v>138</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="5">
         <v>134</v>
       </c>
-      <c r="Y3" s="11">
+      <c r="Y3" s="5">
         <v>132</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Z3" s="5">
         <v>127</v>
       </c>
-      <c r="AA3" s="11">
+      <c r="AA3" s="5">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="1:27" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="3">
         <v>50</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="3">
         <v>40</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="3">
         <v>34</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="3">
         <v>32</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="3">
         <v>29</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="4">
         <v>26</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="4">
         <v>23</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="4">
         <v>21</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="4">
         <v>16</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="14">
         <v>14</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="26">
         <v>11</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="27">
         <v>9</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="27">
         <v>7</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="28">
         <v>5</v>
       </c>
-      <c r="S4" s="10">
+      <c r="S4" s="28">
         <v>1</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="28">
         <v>143</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4" s="28">
         <v>141</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="29">
         <v>139</v>
       </c>
-      <c r="W4" s="15">
+      <c r="W4" s="30">
         <v>137</v>
       </c>
-      <c r="X4" s="11">
+      <c r="X4" s="15">
         <v>133</v>
       </c>
-      <c r="Y4" s="11">
+      <c r="Y4" s="5">
         <v>131</v>
       </c>
-      <c r="Z4" s="11">
+      <c r="Z4" s="5">
         <v>126</v>
       </c>
-      <c r="AA4" s="11">
+      <c r="AA4" s="5">
         <v>123</v>
       </c>
     </row>
+    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="6"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="20">
         <v>58</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="20">
         <v>67</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="20">
         <v>75</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="20">
         <v>79</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="21">
         <v>81</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="21">
         <v>83</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="34">
         <v>85</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="41">
         <v>88</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="42">
         <v>93</v>
       </c>
-      <c r="O14" s="8">
+      <c r="O14" s="42">
         <v>95</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14" s="43">
         <v>98</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14" s="50">
         <v>100</v>
       </c>
-      <c r="R14" s="16">
+      <c r="R14" s="52">
         <v>102</v>
       </c>
-      <c r="S14" s="16">
+      <c r="S14" s="50">
         <v>105</v>
       </c>
-      <c r="T14" s="16">
+      <c r="T14" s="56">
         <v>112</v>
       </c>
-      <c r="U14" s="16">
+      <c r="U14" s="50">
         <v>115</v>
       </c>
-      <c r="V14" s="16">
+      <c r="V14" s="60">
         <v>117</v>
       </c>
-      <c r="W14" s="16">
+      <c r="W14" s="35">
         <v>119</v>
       </c>
-      <c r="X14" s="16">
+      <c r="X14" s="7">
         <v>121</v>
       </c>
-      <c r="Y14" s="7" t="s">
+      <c r="Y14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Z14" s="7" t="s">
+      <c r="Z14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA14" s="7" t="s">
+      <c r="AA14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
+    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="22">
         <v>57</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="23">
         <v>66</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="23">
         <v>74</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="23">
         <v>78</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="24">
         <v>80</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="24">
         <v>82</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="25">
         <v>84</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="36">
         <v>87</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="37">
         <v>92</v>
       </c>
-      <c r="O15" s="8">
+      <c r="O15" s="37">
         <v>94</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="37">
         <v>97</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15" s="7">
         <v>99</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15" s="51">
         <v>101</v>
       </c>
-      <c r="S15" s="16">
+      <c r="S15" s="7">
         <v>104</v>
       </c>
-      <c r="T15" s="16">
+      <c r="T15" s="51">
         <v>111</v>
       </c>
-      <c r="U15" s="16">
+      <c r="U15" s="7">
         <v>114</v>
       </c>
-      <c r="V15" s="16">
+      <c r="V15" s="51">
         <v>116</v>
       </c>
-      <c r="W15" s="16">
+      <c r="W15" s="7">
         <v>118</v>
       </c>
-      <c r="X15" s="16">
+      <c r="X15" s="7">
         <v>120</v>
       </c>
-      <c r="Y15" s="7" t="s">
+      <c r="Y15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Z15" s="7" t="s">
+      <c r="Z15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AA15" s="7" t="s">
+      <c r="AA15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -911,51 +1439,92 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
       <c r="G18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="G19" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="33"/>
+      <c r="L19" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="58"/>
+      <c r="N19" s="59"/>
     </row>
-    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="G20" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40"/>
+      <c r="L20" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="54"/>
+      <c r="N20" s="55"/>
     </row>
-    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
+      <c r="G21" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="46"/>
     </row>
-    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="G22" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="49"/>
     </row>
+    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="L20:N20"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A17:D17"/>
@@ -964,5 +1533,6 @@
     <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>